<commit_message>
added explanation for computing values of Gesamtaufwand of project
</commit_message>
<xml_diff>
--- a/doc/Aufwandserfassung_d6.xlsx
+++ b/doc/Aufwandserfassung_d6.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corinneblessing/Desktop/DHBW Horb Informatik/Semester 4/Software Engineering Project/d6/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{244B0FD8-C13F-EF41-8D01-E7CC6BC48F58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410A4A80-2D47-8944-A0E3-A1141D3B61B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1460" windowWidth="24140" windowHeight="13480" xr2:uid="{5926B423-7E3C-684C-84D4-62A9B5892447}"/>
+    <workbookView xWindow="1120" yWindow="1460" windowWidth="24140" windowHeight="13480" activeTab="1" xr2:uid="{5926B423-7E3C-684C-84D4-62A9B5892447}"/>
   </bookViews>
   <sheets>
-    <sheet name="Wochenaufwand" sheetId="1" r:id="rId1"/>
-    <sheet name="Gesamtaufwand" sheetId="2" r:id="rId2"/>
+    <sheet name="Gesamtaufwand" sheetId="2" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="3" r:id="rId2"/>
+    <sheet name="KW 11" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t xml:space="preserve">Gesamtübersicht Aufwandserfassung Gruppe d6 </t>
   </si>
@@ -178,6 +179,90 @@
   </si>
   <si>
     <t>bis:</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Aufgabe 1</t>
+  </si>
+  <si>
+    <t>Aufgabe 2</t>
+  </si>
+  <si>
+    <t>Aufgabe 3</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>geschätzt</t>
+  </si>
+  <si>
+    <t>tatsächlich</t>
+  </si>
+  <si>
+    <t>Aufwand2</t>
+  </si>
+  <si>
+    <t>Zeitaufwand [in h]</t>
+  </si>
+  <si>
+    <t>Schwierigkeit2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berechnungsgrundlage für den Gesamtaufwand des Projektes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Für die Berechnung werden die tatsächlichen Werte des Aufwandes, der Schwierigkeit und des Zeitumfangs herangezogen. Die Berechnung erfolgt über das arithmetische Mittel. Der Gesamtaufwand während des Betrachtungszeitraums ergibt sich durch die Addition der einzelnen Werte für Aufwand, Schwierigkeit und Zeitumfang und wird durch die Anzahl der erledigten Aufgaben geteilt. </t>
+  </si>
+  <si>
+    <t>Beispiel:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teammitglied 1 reicht folgende Wochenaufwandserfassung ein: </t>
+  </si>
+  <si>
+    <t>Mitglied 1</t>
+  </si>
+  <si>
+    <t>Aufgabe 4</t>
+  </si>
+  <si>
+    <t>Aufgabe 5</t>
+  </si>
+  <si>
+    <t>Aufgabe 6</t>
+  </si>
+  <si>
+    <t>Aufgabe 7</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>XY</t>
+  </si>
+  <si>
+    <t>XZ</t>
+  </si>
+  <si>
+    <t>Aufgabe 8</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die in der gesamten Auswertung errechneten Zeitwerte der tatsächlich ermittelten Werte werden für die Übersicht des Aufwandes während des gesamten Projektes verwendet. </t>
   </si>
 </sst>
 </file>
@@ -252,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -276,15 +361,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -411,28 +487,6 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -640,17 +694,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -658,117 +800,34 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <font>
         <b val="0"/>
@@ -822,9 +881,7 @@
         <left style="medium">
           <color auto="1"/>
         </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -833,6 +890,104 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -993,6 +1148,428 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -1039,9 +1616,9 @@
   <tableStyles count="2" defaultTableStyle="Vorlage Gesamtaufwandserfassung" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Vorlage Aufwandserfassung Gesamt" pivot="0" count="0" xr9:uid="{A575E57F-D35D-5E41-A681-9FCF5B678D6A}"/>
     <tableStyle name="Vorlage Gesamtaufwandserfassung" pivot="0" count="3" xr9:uid="{EBE07CC3-CC63-5947-8161-3FC2D95B76AA}">
-      <tableStyleElement type="wholeTable" dxfId="11"/>
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="firstColumn" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="firstColumn" dxfId="24"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1056,15 +1633,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0ACE7406-0BC3-5F4F-BAF9-B92CE210194D}" name="Tabelle3" displayName="Tabelle3" ref="A11:F16" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="8">
-  <autoFilter ref="A11:F16" xr:uid="{9AC84AAE-FB96-D94A-A829-C3DEF2F9EC0E}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{43B28113-7899-3345-BBCF-FEE3F7472F95}" name="Name" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{24B0E79B-E537-3E4D-8671-16EBE0EB37FF}" name="Arbeitspaket Nr. " dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{D5A9591E-E1FA-B545-BA23-18A474E4F5FC}" name="Aufgabe" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{F7CB1078-1238-F240-8F0D-AB655707846D}" name="Aufwand" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{0DDCB9DD-F69B-4046-89D6-6AFDACD93966}" name="Schwierigkeit" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{CCCB2E79-FB30-B846-A277-29B8487EC67F}" name="Zeitumfang [in h]" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E5414A2-0151-AF49-91FF-FD189A5A2210}" name="Tabelle32" displayName="Tabelle32" ref="B16:J26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="B16:J26" xr:uid="{3FA28FC7-0EA2-A945-9811-B62D149BEFAD}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{B25FCD88-2F9D-8C44-B29E-E46B6C5166B0}" name="Name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{02F79588-7B2B-B14F-B3C3-60259702C400}" name="Arbeitspaket Nr. " dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{006644CB-2C35-0F49-AB75-3E82A2600ADC}" name="Aufgabe" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{8A59437B-1049-1345-B261-D84892EABA48}" name="Aufwand" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{D37CD5E4-ED03-6C4D-9E49-99234BEEA3A9}" name="Aufwand2" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{474CBEC2-2CA9-0F44-A958-1D730AECE932}" name="Schwierigkeit" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{84D443CB-F91A-654F-A53F-EC165426F91A}" name="Schwierigkeit2" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{F63DFBFD-FCAA-AA43-93DC-B14E7CA8EC0C}" name="Zeitaufwand [in h]" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{BFD61E4D-6345-3E44-B2F8-A56318689E44}" name="Zeitumfang [in h]" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="Vorlage Gesamtaufwandserfassung" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0ACE7406-0BC3-5F4F-BAF9-B92CE210194D}" name="Tabelle3" displayName="Tabelle3" ref="A11:I20" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="A11:I20" xr:uid="{9AC84AAE-FB96-D94A-A829-C3DEF2F9EC0E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{43B28113-7899-3345-BBCF-FEE3F7472F95}" name="Name" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{24B0E79B-E537-3E4D-8671-16EBE0EB37FF}" name="Arbeitspaket Nr. " dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{D5A9591E-E1FA-B545-BA23-18A474E4F5FC}" name="Aufgabe" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{708379F8-72D2-594E-BC9A-73FACC3AB6CF}" name="Aufwand" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{F7CB1078-1238-F240-8F0D-AB655707846D}" name="Aufwand2" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{0DDCB9DD-F69B-4046-89D6-6AFDACD93966}" name="Schwierigkeit" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{C63353D8-BAC8-2348-AC06-E9BC67EEFE09}" name="Schwierigkeit2" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{F366E200-830B-DA40-A291-32AB6BB507F8}" name="Zeitaufwand [in h]" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{CCCB2E79-FB30-B846-A277-29B8487EC67F}" name="Zeitumfang [in h]" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Vorlage Gesamtaufwandserfassung" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1366,167 +1964,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D83A78A-74FD-F046-B261-594ED8A74782}">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-    </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="35">
-        <v>43902</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="35">
-        <v>43905</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="37"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="37"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="37"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="37"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="42"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53147F8F-47F5-7645-9070-C97D9B946AB5}">
   <dimension ref="A2:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1538,510 +1980,510 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="2:20" ht="20" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="2:20" ht="20" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="2:20" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="18" t="s">
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="S8" s="18"/>
-      <c r="T8" s="19"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="39"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B9" s="22"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="5" t="s">
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="5" t="s">
+      <c r="J9" s="35"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="6"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15" t="s">
+      <c r="M9" s="35"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="7"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="36"/>
     </row>
     <row r="10" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="13" t="s">
+      <c r="N10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="O10" s="17" t="s">
+      <c r="O10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="17" t="s">
+      <c r="P10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Q10" s="17" t="s">
+      <c r="Q10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="11" t="s">
+      <c r="R10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="S10" s="12" t="s">
+      <c r="S10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="T10" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="22"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="27"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="18"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="10"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="6"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="10"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="6"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="10"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="6"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="10"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="6"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="10"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="6"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="10"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="6"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="10"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="6"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="10"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="6"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="10"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="6"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="10"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="6"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="10"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="6"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="10"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="6"/>
     </row>
     <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="12"/>
-      <c r="T24" s="13"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B25" s="30"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="29"/>
-      <c r="S25" s="29"/>
-      <c r="T25" s="29"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
@@ -2095,16 +2537,810 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C2:G4"/>
+    <mergeCell ref="C8:Q8"/>
+    <mergeCell ref="R8:T8"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="L9:N9"/>
     <mergeCell ref="R9:T9"/>
-    <mergeCell ref="C2:G4"/>
-    <mergeCell ref="C8:Q8"/>
-    <mergeCell ref="R8:T8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1DD99E-BEBD-D74E-B262-5D4089A9699E}">
+  <dimension ref="B2:Q30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="1" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="0.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="37.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="27" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="0.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17" ht="20" x14ac:dyDescent="0.2">
+      <c r="B2" s="49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+    </row>
+    <row r="9" spans="2:17" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+    </row>
+    <row r="10" spans="2:17" ht="5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+    </row>
+    <row r="11" spans="2:17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="26"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="23">
+        <v>1</v>
+      </c>
+      <c r="F18" s="23">
+        <v>2</v>
+      </c>
+      <c r="G18" s="23">
+        <v>1</v>
+      </c>
+      <c r="H18" s="27">
+        <v>2</v>
+      </c>
+      <c r="I18" s="27">
+        <v>1</v>
+      </c>
+      <c r="J18" s="27">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="26"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="23">
+        <v>1</v>
+      </c>
+      <c r="F19" s="23">
+        <v>2</v>
+      </c>
+      <c r="G19" s="23">
+        <v>1</v>
+      </c>
+      <c r="H19" s="27">
+        <v>2</v>
+      </c>
+      <c r="I19" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="26"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="23">
+        <v>1</v>
+      </c>
+      <c r="F20" s="23">
+        <v>1</v>
+      </c>
+      <c r="G20" s="23">
+        <v>1</v>
+      </c>
+      <c r="H20" s="27">
+        <v>1</v>
+      </c>
+      <c r="I20" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J20" s="27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="26"/>
+      <c r="C21" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="23">
+        <v>3</v>
+      </c>
+      <c r="F21" s="23">
+        <v>1</v>
+      </c>
+      <c r="G21" s="23">
+        <v>5</v>
+      </c>
+      <c r="H21" s="27">
+        <v>3</v>
+      </c>
+      <c r="I21" s="27">
+        <v>5</v>
+      </c>
+      <c r="J21" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="26"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="23">
+        <v>2</v>
+      </c>
+      <c r="F22" s="23">
+        <v>1</v>
+      </c>
+      <c r="G22" s="23">
+        <v>4</v>
+      </c>
+      <c r="H22" s="27">
+        <v>1</v>
+      </c>
+      <c r="I22" s="27">
+        <v>2</v>
+      </c>
+      <c r="J22" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="26"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="23">
+        <v>4</v>
+      </c>
+      <c r="F23" s="23">
+        <v>2</v>
+      </c>
+      <c r="G23" s="23">
+        <v>2</v>
+      </c>
+      <c r="H23" s="27">
+        <v>1</v>
+      </c>
+      <c r="I23" s="27">
+        <v>5</v>
+      </c>
+      <c r="J23" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="26"/>
+      <c r="C24" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="23">
+        <v>1</v>
+      </c>
+      <c r="F24" s="23">
+        <v>1</v>
+      </c>
+      <c r="G24" s="23">
+        <v>2</v>
+      </c>
+      <c r="H24" s="27">
+        <v>2</v>
+      </c>
+      <c r="I24" s="27">
+        <v>1</v>
+      </c>
+      <c r="J24" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="31">
+        <v>3</v>
+      </c>
+      <c r="F25" s="31">
+        <v>2</v>
+      </c>
+      <c r="G25" s="31">
+        <v>2</v>
+      </c>
+      <c r="H25" s="32">
+        <v>1</v>
+      </c>
+      <c r="I25" s="32">
+        <v>2</v>
+      </c>
+      <c r="J25" s="32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46">
+        <f>SUM(E18:E25)/8</f>
+        <v>2</v>
+      </c>
+      <c r="F26" s="46">
+        <f>SUM(F18:F25)/8</f>
+        <v>1.5</v>
+      </c>
+      <c r="G26" s="46">
+        <f>SUM(G18:G25)/8</f>
+        <v>2.25</v>
+      </c>
+      <c r="H26" s="47">
+        <f>SUM(H18:H25)/8</f>
+        <v>1.625</v>
+      </c>
+      <c r="I26" s="47">
+        <f>SUM(I18:I25)/8</f>
+        <v>2.125</v>
+      </c>
+      <c r="J26" s="47">
+        <f>SUM(J19:J25)/8</f>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:Q11"/>
+    <mergeCell ref="B29:J30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D83A78A-74FD-F046-B261-594ED8A74782}">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="25">
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="25">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="26"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="27">
+        <v>2</v>
+      </c>
+      <c r="I13" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="26"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="27">
+        <v>4</v>
+      </c>
+      <c r="I14" s="27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="26"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="27">
+        <v>5</v>
+      </c>
+      <c r="I15" s="27">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="26"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F3"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added total expenditure over the week per team member and average of work expenditure
</commit_message>
<xml_diff>
--- a/doc/Aufwandserfassung_d6.xlsx
+++ b/doc/Aufwandserfassung_d6.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corinneblessing/Desktop/DHBW Horb Informatik/Semester 4/Software Engineering Project/d6/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410A4A80-2D47-8944-A0E3-A1141D3B61B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D30C5D-FE31-9F42-9E84-3BB1587E8B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="1460" windowWidth="24140" windowHeight="13480" activeTab="1" xr2:uid="{5926B423-7E3C-684C-84D4-62A9B5892447}"/>
   </bookViews>
   <sheets>
-    <sheet name="Gesamtaufwand" sheetId="2" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="3" r:id="rId2"/>
+    <sheet name="Berechnung Gesamtaufwand" sheetId="3" r:id="rId1"/>
+    <sheet name="Gesamtaufwand" sheetId="2" r:id="rId2"/>
     <sheet name="KW 11" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
-  <si>
-    <t xml:space="preserve">Gesamtübersicht Aufwandserfassung Gruppe d6 </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
   <si>
     <t>Corinne Blessing</t>
   </si>
@@ -193,15 +190,6 @@
     <t>Aufgabe 3</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>geschätzt</t>
   </si>
   <si>
@@ -217,9 +205,6 @@
     <t>Schwierigkeit2</t>
   </si>
   <si>
-    <t xml:space="preserve">b </t>
-  </si>
-  <si>
     <t xml:space="preserve">Berechnungsgrundlage für den Gesamtaufwand des Projektes </t>
   </si>
   <si>
@@ -263,6 +248,24 @@
   </si>
   <si>
     <t xml:space="preserve">Die in der gesamten Auswertung errechneten Zeitwerte der tatsächlich ermittelten Werte werden für die Übersicht des Aufwandes während des gesamten Projektes verwendet. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesamtübersicht Aufwandserfassung KW 11 Gruppe d6 </t>
+  </si>
+  <si>
+    <t>Wochenüberblick</t>
+  </si>
+  <si>
+    <t>Abweichung [in %]</t>
+  </si>
+  <si>
+    <t>Durchschnittliche Arbeitsleistung im Team</t>
+  </si>
+  <si>
+    <t>Erbrachte Arbeitsleistung des Teams [in h]</t>
+  </si>
+  <si>
+    <t>Erbrachte Stunden</t>
   </si>
 </sst>
 </file>
@@ -337,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -740,11 +743,133 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -788,8 +913,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -800,29 +948,64 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1283,6 +1466,38 @@
         <left style="medium">
           <color auto="1"/>
         </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
         <right style="medium">
           <color auto="1"/>
         </right>
@@ -1326,38 +1541,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1633,36 +1816,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E5414A2-0151-AF49-91FF-FD189A5A2210}" name="Tabelle32" displayName="Tabelle32" ref="B16:J26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E5414A2-0151-AF49-91FF-FD189A5A2210}" name="Tabelle32" displayName="Tabelle32" ref="B16:J26" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="B16:J26" xr:uid="{3FA28FC7-0EA2-A945-9811-B62D149BEFAD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B25FCD88-2F9D-8C44-B29E-E46B6C5166B0}" name="Name" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{02F79588-7B2B-B14F-B3C3-60259702C400}" name="Arbeitspaket Nr. " dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{006644CB-2C35-0F49-AB75-3E82A2600ADC}" name="Aufgabe" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{8A59437B-1049-1345-B261-D84892EABA48}" name="Aufwand" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{D37CD5E4-ED03-6C4D-9E49-99234BEEA3A9}" name="Aufwand2" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{474CBEC2-2CA9-0F44-A958-1D730AECE932}" name="Schwierigkeit" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{84D443CB-F91A-654F-A53F-EC165426F91A}" name="Schwierigkeit2" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{F63DFBFD-FCAA-AA43-93DC-B14E7CA8EC0C}" name="Zeitaufwand [in h]" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{BFD61E4D-6345-3E44-B2F8-A56318689E44}" name="Zeitumfang [in h]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B25FCD88-2F9D-8C44-B29E-E46B6C5166B0}" name="Name" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{02F79588-7B2B-B14F-B3C3-60259702C400}" name="Arbeitspaket Nr. " dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{006644CB-2C35-0F49-AB75-3E82A2600ADC}" name="Aufgabe" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{8A59437B-1049-1345-B261-D84892EABA48}" name="Aufwand" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{D37CD5E4-ED03-6C4D-9E49-99234BEEA3A9}" name="Aufwand2" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{474CBEC2-2CA9-0F44-A958-1D730AECE932}" name="Schwierigkeit" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{84D443CB-F91A-654F-A53F-EC165426F91A}" name="Schwierigkeit2" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{F63DFBFD-FCAA-AA43-93DC-B14E7CA8EC0C}" name="Zeitaufwand [in h]" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{BFD61E4D-6345-3E44-B2F8-A56318689E44}" name="Zeitumfang [in h]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="Vorlage Gesamtaufwandserfassung" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0ACE7406-0BC3-5F4F-BAF9-B92CE210194D}" name="Tabelle3" displayName="Tabelle3" ref="A11:I20" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0ACE7406-0BC3-5F4F-BAF9-B92CE210194D}" name="Tabelle3" displayName="Tabelle3" ref="A11:I20" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A11:I20" xr:uid="{9AC84AAE-FB96-D94A-A829-C3DEF2F9EC0E}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{43B28113-7899-3345-BBCF-FEE3F7472F95}" name="Name" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{24B0E79B-E537-3E4D-8671-16EBE0EB37FF}" name="Arbeitspaket Nr. " dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{D5A9591E-E1FA-B545-BA23-18A474E4F5FC}" name="Aufgabe" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{708379F8-72D2-594E-BC9A-73FACC3AB6CF}" name="Aufwand" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{F7CB1078-1238-F240-8F0D-AB655707846D}" name="Aufwand2" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{0DDCB9DD-F69B-4046-89D6-6AFDACD93966}" name="Schwierigkeit" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{C63353D8-BAC8-2348-AC06-E9BC67EEFE09}" name="Schwierigkeit2" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{F366E200-830B-DA40-A291-32AB6BB507F8}" name="Zeitaufwand [in h]" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{CCCB2E79-FB30-B846-A277-29B8487EC67F}" name="Zeitumfang [in h]" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{43B28113-7899-3345-BBCF-FEE3F7472F95}" name="Name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{24B0E79B-E537-3E4D-8671-16EBE0EB37FF}" name="Arbeitspaket Nr. " dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{D5A9591E-E1FA-B545-BA23-18A474E4F5FC}" name="Aufgabe" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{708379F8-72D2-594E-BC9A-73FACC3AB6CF}" name="Aufwand" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{F7CB1078-1238-F240-8F0D-AB655707846D}" name="Aufwand2" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{0DDCB9DD-F69B-4046-89D6-6AFDACD93966}" name="Schwierigkeit" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{C63353D8-BAC8-2348-AC06-E9BC67EEFE09}" name="Schwierigkeit2" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{F366E200-830B-DA40-A291-32AB6BB507F8}" name="Zeitaufwand [in h]" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{CCCB2E79-FB30-B846-A277-29B8487EC67F}" name="Zeitumfang [in h]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Vorlage Gesamtaufwandserfassung" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1964,599 +2147,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53147F8F-47F5-7645-9070-C97D9B946AB5}">
-  <dimension ref="A2:T31"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" customWidth="1"/>
-    <col min="3" max="17" width="8.83203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C2" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-    </row>
-    <row r="5" spans="2:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="2:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="2:20" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="S8" s="38"/>
-      <c r="T8" s="39"/>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
-      <c r="C9" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="35"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="36"/>
-    </row>
-    <row r="10" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="T10" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="18"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="6"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="6"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="6"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B15" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="6"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="6"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B17" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="6"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="6"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B19" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="6"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B20" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="6"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B21" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="6"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="6"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B23" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="6"/>
-    </row>
-    <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="9"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B25" s="20"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C2:G4"/>
-    <mergeCell ref="C8:Q8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R9:T9"/>
-  </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1DD99E-BEBD-D74E-B262-5D4089A9699E}">
   <dimension ref="B2:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -2578,69 +2172,548 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+    </row>
+    <row r="9" spans="2:17" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+    </row>
+    <row r="10" spans="2:17" ht="5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+    </row>
+    <row r="11" spans="2:17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="26"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="23">
+        <v>1</v>
+      </c>
+      <c r="F18" s="23">
+        <v>2</v>
+      </c>
+      <c r="G18" s="23">
+        <v>1</v>
+      </c>
+      <c r="H18" s="27">
+        <v>2</v>
+      </c>
+      <c r="I18" s="27">
+        <v>1</v>
+      </c>
+      <c r="J18" s="27">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="26"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="23">
+        <v>1</v>
+      </c>
+      <c r="F19" s="23">
+        <v>2</v>
+      </c>
+      <c r="G19" s="23">
+        <v>1</v>
+      </c>
+      <c r="H19" s="27">
+        <v>2</v>
+      </c>
+      <c r="I19" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="26"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="23">
+        <v>1</v>
+      </c>
+      <c r="F20" s="23">
+        <v>1</v>
+      </c>
+      <c r="G20" s="23">
+        <v>1</v>
+      </c>
+      <c r="H20" s="27">
+        <v>1</v>
+      </c>
+      <c r="I20" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J20" s="27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="26"/>
+      <c r="C21" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+      <c r="E21" s="23">
+        <v>3</v>
+      </c>
+      <c r="F21" s="23">
+        <v>1</v>
+      </c>
+      <c r="G21" s="23">
+        <v>5</v>
+      </c>
+      <c r="H21" s="27">
+        <v>3</v>
+      </c>
+      <c r="I21" s="27">
+        <v>5</v>
+      </c>
+      <c r="J21" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="26"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="44"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="E22" s="23">
+        <v>2</v>
+      </c>
+      <c r="F22" s="23">
+        <v>1</v>
+      </c>
+      <c r="G22" s="23">
+        <v>4</v>
+      </c>
+      <c r="H22" s="27">
+        <v>1</v>
+      </c>
+      <c r="I22" s="27">
+        <v>2</v>
+      </c>
+      <c r="J22" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="26"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="23">
+        <v>4</v>
+      </c>
+      <c r="F23" s="23">
+        <v>2</v>
+      </c>
+      <c r="G23" s="23">
+        <v>2</v>
+      </c>
+      <c r="H23" s="27">
+        <v>1</v>
+      </c>
+      <c r="I23" s="27">
+        <v>5</v>
+      </c>
+      <c r="J23" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="26"/>
+      <c r="C24" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="23">
+        <v>1</v>
+      </c>
+      <c r="F24" s="23">
+        <v>1</v>
+      </c>
+      <c r="G24" s="23">
+        <v>2</v>
+      </c>
+      <c r="H24" s="27">
+        <v>2</v>
+      </c>
+      <c r="I24" s="27">
+        <v>1</v>
+      </c>
+      <c r="J24" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="31">
+        <v>3</v>
+      </c>
+      <c r="F25" s="31">
+        <v>2</v>
+      </c>
+      <c r="G25" s="31">
+        <v>2</v>
+      </c>
+      <c r="H25" s="32">
+        <v>1</v>
+      </c>
+      <c r="I25" s="32">
+        <v>2</v>
+      </c>
+      <c r="J25" s="32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38">
+        <f>SUM(E18:E25)/8</f>
+        <v>2</v>
+      </c>
+      <c r="F26" s="38">
+        <f>SUM(F18:F25)/8</f>
+        <v>1.5</v>
+      </c>
+      <c r="G26" s="38">
+        <f>SUM(G18:G25)/8</f>
+        <v>2.25</v>
+      </c>
+      <c r="H26" s="39">
+        <f>SUM(H18:H25)/8</f>
+        <v>1.625</v>
+      </c>
+      <c r="I26" s="39">
+        <f>SUM(I18:I25)/8</f>
+        <v>2.125</v>
+      </c>
+      <c r="J26" s="39">
+        <f>SUM(J19:J25)/8</f>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:Q11"/>
+    <mergeCell ref="B29:J30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53147F8F-47F5-7645-9070-C97D9B946AB5}">
+  <dimension ref="A2:T31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" customWidth="1"/>
+    <col min="3" max="17" width="8.83203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C2" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+    </row>
+    <row r="5" spans="2:20" ht="20" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="2:20" ht="20" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="2:20" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>37</v>
+      </c>
       <c r="D8" s="44"/>
       <c r="E8" s="44"/>
       <c r="F8" s="44"/>
@@ -2655,404 +2728,514 @@
       <c r="O8" s="44"/>
       <c r="P8" s="44"/>
       <c r="Q8" s="44"/>
-    </row>
-    <row r="9" spans="2:17" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-    </row>
-    <row r="10" spans="2:17" ht="5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-    </row>
-    <row r="11" spans="2:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B16" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="28" t="s">
+      <c r="R8" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="45"/>
+      <c r="T8" s="46"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="13"/>
+      <c r="C9" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="48"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="48"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="48"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="49"/>
+    </row>
+    <row r="10" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="13"/>
+      <c r="C10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B11" s="13"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="18"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="6"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="6"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="6"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="6"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="6"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="6"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="6"/>
+    </row>
+    <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="9"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B25" s="20"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="28" t="s">
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="26"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="J17" s="41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="23">
-        <v>1</v>
-      </c>
-      <c r="F18" s="23">
-        <v>2</v>
-      </c>
-      <c r="G18" s="23">
-        <v>1</v>
-      </c>
-      <c r="H18" s="27">
-        <v>2</v>
-      </c>
-      <c r="I18" s="27">
-        <v>1</v>
-      </c>
-      <c r="J18" s="27">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="26"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="23">
-        <v>1</v>
-      </c>
-      <c r="F19" s="23">
-        <v>2</v>
-      </c>
-      <c r="G19" s="23">
-        <v>1</v>
-      </c>
-      <c r="H19" s="27">
-        <v>2</v>
-      </c>
-      <c r="I19" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="J19" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="26"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="23">
-        <v>1</v>
-      </c>
-      <c r="F20" s="23">
-        <v>1</v>
-      </c>
-      <c r="G20" s="23">
-        <v>1</v>
-      </c>
-      <c r="H20" s="27">
-        <v>1</v>
-      </c>
-      <c r="I20" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="J20" s="27">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="26"/>
-      <c r="C21" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="23">
-        <v>3</v>
-      </c>
-      <c r="F21" s="23">
-        <v>1</v>
-      </c>
-      <c r="G21" s="23">
-        <v>5</v>
-      </c>
-      <c r="H21" s="27">
-        <v>3</v>
-      </c>
-      <c r="I21" s="27">
-        <v>5</v>
-      </c>
-      <c r="J21" s="27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="26"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="23">
-        <v>2</v>
-      </c>
-      <c r="F22" s="23">
-        <v>1</v>
-      </c>
-      <c r="G22" s="23">
-        <v>4</v>
-      </c>
-      <c r="H22" s="27">
-        <v>1</v>
-      </c>
-      <c r="I22" s="27">
-        <v>2</v>
-      </c>
-      <c r="J22" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="26"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="23">
-        <v>4</v>
-      </c>
-      <c r="F23" s="23">
-        <v>2</v>
-      </c>
-      <c r="G23" s="23">
-        <v>2</v>
-      </c>
-      <c r="H23" s="27">
-        <v>1</v>
-      </c>
-      <c r="I23" s="27">
-        <v>5</v>
-      </c>
-      <c r="J23" s="27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="26"/>
-      <c r="C24" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="23">
-        <v>1</v>
-      </c>
-      <c r="F24" s="23">
-        <v>1</v>
-      </c>
-      <c r="G24" s="23">
-        <v>2</v>
-      </c>
-      <c r="H24" s="27">
-        <v>2</v>
-      </c>
-      <c r="I24" s="27">
-        <v>1</v>
-      </c>
-      <c r="J24" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="31">
-        <v>3</v>
-      </c>
-      <c r="F25" s="31">
-        <v>2</v>
-      </c>
-      <c r="G25" s="31">
-        <v>2</v>
-      </c>
-      <c r="H25" s="32">
-        <v>1</v>
-      </c>
-      <c r="I25" s="32">
-        <v>2</v>
-      </c>
-      <c r="J25" s="32">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46">
-        <f>SUM(E18:E25)/8</f>
-        <v>2</v>
-      </c>
-      <c r="F26" s="46">
-        <f>SUM(F18:F25)/8</f>
-        <v>1.5</v>
-      </c>
-      <c r="G26" s="46">
-        <f>SUM(G18:G25)/8</f>
-        <v>2.25</v>
-      </c>
-      <c r="H26" s="47">
-        <f>SUM(H18:H25)/8</f>
-        <v>1.625</v>
-      </c>
-      <c r="I26" s="47">
-        <f>SUM(I18:I25)/8</f>
-        <v>2.125</v>
-      </c>
-      <c r="J26" s="47">
-        <f>SUM(J19:J25)/8</f>
-        <v>1.375</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B5:Q11"/>
-    <mergeCell ref="B29:J30"/>
+  <mergeCells count="8">
+    <mergeCell ref="C2:G4"/>
+    <mergeCell ref="C8:Q8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R9:T9"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D83A78A-74FD-F046-B261-594ED8A74782}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H33" sqref="H33:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3069,31 +3252,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
     </row>
@@ -3117,15 +3300,15 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="25">
         <v>43902</v>
@@ -3133,7 +3316,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="25">
         <v>43905</v>
@@ -3141,77 +3324,77 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="E11" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="28" t="s">
+      <c r="G11" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="29" t="s">
         <v>10</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="26"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="41" t="s">
-        <v>56</v>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="71" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>54</v>
+      <c r="D13" s="23">
+        <v>1</v>
+      </c>
+      <c r="E13" s="23">
+        <v>2</v>
+      </c>
+      <c r="F13" s="23">
+        <v>1</v>
+      </c>
+      <c r="G13" s="27">
+        <v>3</v>
       </c>
       <c r="H13" s="27">
         <v>2</v>
@@ -3224,19 +3407,19 @@
       <c r="A14" s="26"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="D14" s="23">
+        <v>2</v>
+      </c>
+      <c r="E14" s="23">
+        <v>3</v>
+      </c>
+      <c r="F14" s="23">
+        <v>2</v>
+      </c>
+      <c r="G14" s="27">
+        <v>3</v>
       </c>
       <c r="H14" s="27">
         <v>4</v>
@@ -3249,19 +3432,19 @@
       <c r="A15" s="26"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="D15" s="23">
+        <v>3</v>
+      </c>
+      <c r="E15" s="23">
+        <v>1</v>
+      </c>
+      <c r="F15" s="23">
+        <v>3</v>
+      </c>
+      <c r="G15" s="27">
+        <v>2</v>
       </c>
       <c r="H15" s="27">
         <v>5</v>
@@ -3283,7 +3466,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -3296,7 +3479,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
@@ -3309,7 +3492,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -3322,7 +3505,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
@@ -3333,9 +3516,157 @@
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
     </row>
+    <row r="23" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="A23" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+    </row>
+    <row r="24" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+    </row>
+    <row r="25" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="60"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="61"/>
+      <c r="B26" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="73" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="75"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="76">
+        <f>SUM(D13:D20)</f>
+        <v>6</v>
+      </c>
+      <c r="C27" s="77">
+        <f>SUM(E13:E20)</f>
+        <v>6</v>
+      </c>
+      <c r="D27" s="78">
+        <v>0</v>
+      </c>
+      <c r="E27" s="79"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="76">
+        <f>SUM(F13:F20)</f>
+        <v>6</v>
+      </c>
+      <c r="C28" s="77">
+        <f>SUM(G13:G20)</f>
+        <v>8</v>
+      </c>
+      <c r="D28" s="78">
+        <f>(B28-C28)/B28</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="E28" s="79"/>
+    </row>
+    <row r="29" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="80">
+        <f>SUM(H13:H20)</f>
+        <v>11</v>
+      </c>
+      <c r="C29" s="81">
+        <f>SUM(I13:I20)</f>
+        <v>11.5</v>
+      </c>
+      <c r="D29" s="82">
+        <f>(B29-C29)/B29</f>
+        <v>-4.5454545454545456E-2</v>
+      </c>
+      <c r="E29" s="83"/>
+    </row>
+    <row r="30" spans="1:9" ht="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="54"/>
+    </row>
+    <row r="31" spans="1:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="67"/>
+    </row>
+    <row r="32" spans="1:9" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="54"/>
+    </row>
+    <row r="33" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="55">
+        <f>SUM(I13:I20)</f>
+        <v>11.5</v>
+      </c>
+      <c r="C33" s="55"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="57"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="7">
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A25:E25"/>
     <mergeCell ref="B1:F3"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>